<commit_message>
Added vias and traces for better connection between two layers and the 12 V line
</commit_message>
<xml_diff>
--- a/Sparrow_V200LF_BOM.xlsx
+++ b/Sparrow_V200LF_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pollock\Documents\Repo\hardware_sparrow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55FB276-E982-4083-8CC2-B1F1B57D0861}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4C215C-48ED-46AF-BD43-F9C8539800E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6BB6B917-AF56-4B92-AD82-C7250C129153}"/>
   </bookViews>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -552,6 +555,11 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -561,11 +569,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -884,7 +887,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,19 +904,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="33"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1061,7 +1064,7 @@
       <c r="J6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="34" t="s">
+      <c r="K6" s="31" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1098,7 +1101,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="35">
+      <c r="A8" s="32">
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1127,7 +1130,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="35">
+      <c r="A9" s="32">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1189,7 +1192,7 @@
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="36">
+      <c r="A11" s="33">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1253,7 +1256,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="36">
+      <c r="A13" s="33">
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1288,7 +1291,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="36">
+      <c r="A14" s="33">
         <v>12</v>
       </c>
       <c r="B14" s="24" t="s">

</xml_diff>

<commit_message>
After PCB Check by Ovee
</commit_message>
<xml_diff>
--- a/Sparrow_V200LF_BOM.xlsx
+++ b/Sparrow_V200LF_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pollock\Documents\Repo\hardware_sparrow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4C215C-48ED-46AF-BD43-F9C8539800E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F88CC2-9D0D-43B3-9418-9AFCC213EE6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6BB6B917-AF56-4B92-AD82-C7250C129153}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t>Qty</t>
   </si>
@@ -222,15 +222,6 @@
     <t>0805</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>2.2 uH</t>
-  </si>
-  <si>
-    <t>Inductor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Espressif </t>
   </si>
   <si>
@@ -249,19 +240,7 @@
     <t>5V Input, 3.3V Output</t>
   </si>
   <si>
-    <t>Coilcraft</t>
-  </si>
-  <si>
-    <t>XFL4020-222MEB</t>
-  </si>
-  <si>
-    <t>3.1-A, 0.165-in × 0.165-in (4.19-mm × 4.19-mm)</t>
-  </si>
-  <si>
     <t>https://my.mouser.com/ProductDetail/STMicroelectronics/LD1117S33TR?qs=%2Fha2pyFaduia9VwYkVWx%2F4mRyX5zUinnP5LH1XIijR0%3D</t>
-  </si>
-  <si>
-    <t>https://my.mouser.com/ProductDetail/Coilcraft/XFL4020-222MEB?qs=%2Fha2pyFaduigLhcKZCbSe3elLWzcz4lGNhw%2F5wHoyzO7kf5YcM2LwA%3D%3D</t>
   </si>
   <si>
     <t>https://www.aliexpress.com/item/4001076646006.html?spm=a2g0o.productlist.0.0.3d3d748a94fsMU&amp;algo_pvid=3e34435e-c6fa-4900-a290-9ef20709fcb8&amp;algo_expid=3e34435e-c6fa-4900-a290-9ef20709fcb8-2&amp;btsid=0bb0623216113166336288081edf43&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_</t>
@@ -376,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -450,15 +429,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -477,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -549,9 +519,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -559,7 +526,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -884,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99144AAD-22C5-4B4D-A92C-45347D70963E}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -904,19 +871,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="36"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -1064,118 +1031,115 @@
       <c r="J6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="31" t="s">
-        <v>76</v>
+      <c r="K6" s="30" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="24">
+      <c r="B7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="8">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" t="s">
-        <v>72</v>
-      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
       <c r="F7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="17">
+        <v>2</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="32">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="23" t="s">
-        <v>57</v>
+      <c r="J8" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="32">
+      <c r="A9" s="31">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="17">
-        <v>2</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" s="14" t="s">
+      <c r="B9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="8">
+        <v>5</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>49</v>
-      </c>
+      <c r="J9" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="C10" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="9" t="s">
-        <v>12</v>
+      <c r="F10" s="11" t="s">
+        <v>16</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>14</v>
@@ -1192,141 +1156,112 @@
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="33">
+      <c r="A11" s="32">
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C11" s="8">
         <v>1</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>61</v>
+      <c r="D11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="9"/>
+      <c r="J11" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C12" s="8">
         <v>1</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>25</v>
+      <c r="D12" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>39</v>
+      <c r="J12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="33">
+      <c r="A13" s="32">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="8">
+      <c r="B13" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="24">
         <v>1</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>60</v>
-      </c>
       <c r="H13" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="20" t="s">
-        <v>29</v>
-      </c>
       <c r="K13" s="23" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="33">
-        <v>12</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="24">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="H14" t="s">
         <v>66</v>
       </c>
-      <c r="F14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H15" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" s="30" t="s">
+      <c r="I14" s="29" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1336,15 +1271,14 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K8" r:id="rId1" display="https://www.digikey.my/product-detail/en/molex/1050170001/WM1399CT-ND/2350885?utm_adgroup=Molex&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Supplier&amp;utm_term=&amp;productid=&amp;gclid=Cj0KCQjwirz3BRD_ARIsAImf7LN2gszsfY4YytdwDBAgQIgrsk3-NnYL0r1gYOgbd5p5W7NCgwE0Uh8aAmPcEALw_wcB" xr:uid="{731BEBB3-6FC4-4C1C-85B2-3B270801C9D9}"/>
-    <hyperlink ref="K13" r:id="rId2" xr:uid="{C7E18DA1-AB1B-4870-95CC-F1AEB2C4B505}"/>
-    <hyperlink ref="K9" r:id="rId3" xr:uid="{8F5B734F-98EB-4104-87F4-EB7B2306BF45}"/>
-    <hyperlink ref="D9" r:id="rId4" display="https://www.digikey.my/en/supplier-centers/o/on-semiconductor" xr:uid="{DE11E3BD-6DBB-41C3-AB24-67D195ECE2F6}"/>
-    <hyperlink ref="K14" r:id="rId5" xr:uid="{E0BBD506-823B-486F-803A-5D3244F08A6D}"/>
-    <hyperlink ref="K7" r:id="rId6" xr:uid="{592EAFF6-9CFF-48D7-9034-B4349D461F5D}"/>
-    <hyperlink ref="K6" r:id="rId7" display="https://www.aliexpress.com/item/4001076646006.html?spm=a2g0o.productlist.0.0.3d3d748a94fsMU&amp;algo_pvid=3e34435e-c6fa-4900-a290-9ef20709fcb8&amp;algo_expid=3e34435e-c6fa-4900-a290-9ef20709fcb8-2&amp;btsid=0bb0623216113166336288081edf43&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_" xr:uid="{FAAF2948-437D-4840-B5FE-39E0E64BE873}"/>
+    <hyperlink ref="K7" r:id="rId1" display="https://www.digikey.my/product-detail/en/molex/1050170001/WM1399CT-ND/2350885?utm_adgroup=Molex&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Supplier&amp;utm_term=&amp;productid=&amp;gclid=Cj0KCQjwirz3BRD_ARIsAImf7LN2gszsfY4YytdwDBAgQIgrsk3-NnYL0r1gYOgbd5p5W7NCgwE0Uh8aAmPcEALw_wcB" xr:uid="{731BEBB3-6FC4-4C1C-85B2-3B270801C9D9}"/>
+    <hyperlink ref="K12" r:id="rId2" xr:uid="{C7E18DA1-AB1B-4870-95CC-F1AEB2C4B505}"/>
+    <hyperlink ref="K8" r:id="rId3" xr:uid="{8F5B734F-98EB-4104-87F4-EB7B2306BF45}"/>
+    <hyperlink ref="D8" r:id="rId4" display="https://www.digikey.my/en/supplier-centers/o/on-semiconductor" xr:uid="{DE11E3BD-6DBB-41C3-AB24-67D195ECE2F6}"/>
+    <hyperlink ref="K13" r:id="rId5" xr:uid="{E0BBD506-823B-486F-803A-5D3244F08A6D}"/>
+    <hyperlink ref="K6" r:id="rId6" display="https://www.aliexpress.com/item/4001076646006.html?spm=a2g0o.productlist.0.0.3d3d748a94fsMU&amp;algo_pvid=3e34435e-c6fa-4900-a290-9ef20709fcb8&amp;algo_expid=3e34435e-c6fa-4900-a290-9ef20709fcb8-2&amp;btsid=0bb0623216113166336288081edf43&amp;ws_ab_test=searchweb0_0,searchweb201602_,searchweb201603_" xr:uid="{FAAF2948-437D-4840-B5FE-39E0E64BE873}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>